<commit_message>
switch pap end to L1, remake figures to reflect this
</commit_message>
<xml_diff>
--- a/tables/supplementary_table_2.xlsx
+++ b/tables/supplementary_table_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonmifsud/Documents/GitHub/phd/p5_marine_mammal/manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonmifsud/Documents/GitHub/phd/p5_marine_mammal/npj_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5DA4D-3277-5848-91D3-CCB26DD40D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD48302-5B12-B44F-A56A-0241991A00DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="2520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supplementary_domains" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="61">
   <si>
     <t>Sequence</t>
   </si>
@@ -201,6 +201,21 @@
   </si>
   <si>
     <t>Supplementary Table 2. Predicted ORFs, protein products and binding sites</t>
+  </si>
+  <si>
+    <t>DNA-dependent DNA polymerase</t>
+  </si>
+  <si>
+    <t>DNA-dependent DNA polymerase (PTHR10322)</t>
+  </si>
+  <si>
+    <t>dUTPase protein</t>
+  </si>
+  <si>
+    <t>dUTPase protein (PF04797)</t>
+  </si>
+  <si>
+    <t>PANTHER</t>
   </si>
 </sst>
 </file>
@@ -536,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -666,6 +681,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -711,11 +750,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -761,7 +806,31 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -775,17 +844,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:H39" totalsRowShown="0">
-  <autoFilter ref="A2:H39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:H43" totalsRowShown="0">
+  <autoFilter ref="A2:H43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sequence"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Minimum"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Maximum"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Length"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="# Intervals"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Database"/>
+    <tableColumn id="6" xr3:uid="{A3748D00-068E-0E48-89E5-D7FB947541BB}" name="Length" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{132C9AA5-C440-BA46-92CA-A3AF8B81BFCB}" name="# Intervals" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{CA106DEF-FAD3-D143-AAB3-5E16D0B6649C}" name="Database"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1088,13 +1157,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" customWidth="1"/>
@@ -1143,10 +1215,10 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>432</v>
       </c>
       <c r="E3">
-        <v>412</v>
+        <v>843</v>
       </c>
       <c r="F3">
         <v>412</v>
@@ -1169,10 +1241,10 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>432</v>
       </c>
       <c r="E4">
-        <v>435</v>
+        <v>866</v>
       </c>
       <c r="F4">
         <v>435</v>
@@ -1195,10 +1267,10 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>73</v>
+        <v>504</v>
       </c>
       <c r="E5">
-        <v>402</v>
+        <v>833</v>
       </c>
       <c r="F5">
         <v>222</v>
@@ -1221,10 +1293,10 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>410</v>
+        <v>841</v>
       </c>
       <c r="E6">
-        <v>700</v>
+        <v>1131</v>
       </c>
       <c r="F6">
         <v>291</v>
@@ -1247,10 +1319,10 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>413</v>
+        <v>844</v>
       </c>
       <c r="E7">
-        <v>668</v>
+        <v>1099</v>
       </c>
       <c r="F7">
         <v>256</v>
@@ -1273,10 +1345,10 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>687</v>
+        <v>1118</v>
       </c>
       <c r="E8">
-        <v>2507</v>
+        <v>2012</v>
       </c>
       <c r="F8">
         <v>1821</v>
@@ -1299,13 +1371,13 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>687</v>
+        <v>1118</v>
       </c>
       <c r="E9">
-        <v>3873</v>
+        <v>2012</v>
       </c>
       <c r="F9">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -1325,10 +1397,10 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <v>690</v>
+        <v>1121</v>
       </c>
       <c r="E10">
-        <v>2505</v>
+        <v>2012</v>
       </c>
       <c r="F10">
         <v>1816</v>
@@ -1351,10 +1423,10 @@
         <v>23</v>
       </c>
       <c r="D11">
-        <v>1026</v>
+        <v>1457</v>
       </c>
       <c r="E11">
-        <v>1040</v>
+        <v>2012</v>
       </c>
       <c r="F11">
         <v>15</v>
@@ -1377,13 +1449,13 @@
         <v>24</v>
       </c>
       <c r="D12">
-        <v>1072</v>
+        <v>1503</v>
       </c>
       <c r="E12">
-        <v>3873</v>
+        <v>2012</v>
       </c>
       <c r="F12">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1403,7 +1475,7 @@
         <v>25</v>
       </c>
       <c r="D13">
-        <v>1989</v>
+        <v>2421</v>
       </c>
       <c r="E13">
         <v>2012</v>
@@ -1429,10 +1501,10 @@
         <v>26</v>
       </c>
       <c r="D14">
-        <v>2449</v>
+        <v>2880</v>
       </c>
       <c r="E14">
-        <v>3873</v>
+        <v>4304</v>
       </c>
       <c r="F14">
         <v>1425</v>
@@ -1455,10 +1527,10 @@
         <v>27</v>
       </c>
       <c r="D15">
-        <v>2452</v>
+        <v>2883</v>
       </c>
       <c r="E15">
-        <v>3805</v>
+        <v>4236</v>
       </c>
       <c r="F15">
         <v>1354</v>
@@ -1481,10 +1553,10 @@
         <v>28</v>
       </c>
       <c r="D16">
-        <v>4402</v>
+        <v>4833</v>
       </c>
       <c r="E16">
-        <v>5937</v>
+        <v>6368</v>
       </c>
       <c r="F16">
         <v>1536</v>
@@ -1507,10 +1579,10 @@
         <v>29</v>
       </c>
       <c r="D17">
-        <v>4405</v>
+        <v>4836</v>
       </c>
       <c r="E17">
-        <v>5935</v>
+        <v>6366</v>
       </c>
       <c r="F17">
         <v>1531</v>
@@ -1533,13 +1605,13 @@
         <v>30</v>
       </c>
       <c r="D18">
-        <v>5957</v>
+        <v>6388</v>
       </c>
       <c r="E18">
-        <v>7496</v>
+        <v>7926</v>
       </c>
       <c r="F18">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1559,10 +1631,10 @@
         <v>31</v>
       </c>
       <c r="D19">
-        <v>5969</v>
+        <v>6400</v>
       </c>
       <c r="E19">
-        <v>7358</v>
+        <v>7789</v>
       </c>
       <c r="F19">
         <v>1390</v>
@@ -1585,13 +1657,13 @@
         <v>34</v>
       </c>
       <c r="D20">
-        <v>7497</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>7926</v>
+        <v>431</v>
       </c>
       <c r="F20">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1611,10 +1683,10 @@
         <v>35</v>
       </c>
       <c r="D21">
-        <v>7634</v>
+        <v>139</v>
       </c>
       <c r="E21">
-        <v>7645</v>
+        <v>150</v>
       </c>
       <c r="F21">
         <v>12</v>
@@ -1637,10 +1709,10 @@
         <v>36</v>
       </c>
       <c r="D22">
-        <v>7695</v>
+        <v>200</v>
       </c>
       <c r="E22">
-        <v>7710</v>
+        <v>215</v>
       </c>
       <c r="F22">
         <v>16</v>
@@ -1663,10 +1735,10 @@
         <v>37</v>
       </c>
       <c r="D23">
-        <v>7754</v>
+        <v>259</v>
       </c>
       <c r="E23">
-        <v>7758</v>
+        <v>263</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -1689,10 +1761,10 @@
         <v>38</v>
       </c>
       <c r="D24">
-        <v>7780</v>
+        <v>285</v>
       </c>
       <c r="E24">
-        <v>7791</v>
+        <v>296</v>
       </c>
       <c r="F24">
         <v>12</v>
@@ -1715,10 +1787,10 @@
         <v>39</v>
       </c>
       <c r="D25">
-        <v>7835</v>
+        <v>340</v>
       </c>
       <c r="E25">
-        <v>7849</v>
+        <v>354</v>
       </c>
       <c r="F25">
         <v>15</v>
@@ -1741,10 +1813,10 @@
         <v>40</v>
       </c>
       <c r="D26">
-        <v>7874</v>
+        <v>379</v>
       </c>
       <c r="E26">
-        <v>7885</v>
+        <v>390</v>
       </c>
       <c r="F26">
         <v>12</v>
@@ -1767,10 +1839,10 @@
         <v>41</v>
       </c>
       <c r="D27">
-        <v>7889</v>
+        <v>394</v>
       </c>
       <c r="E27">
-        <v>7892</v>
+        <v>397</v>
       </c>
       <c r="F27">
         <v>4</v>
@@ -1799,7 +1871,7 @@
         <v>4547</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F36" si="0">E28-D28+1</f>
+        <f>E28-D28+1</f>
         <v>4239</v>
       </c>
       <c r="G28" s="1">
@@ -1826,7 +1898,7 @@
         <v>4524</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f>E29-D29+1</f>
         <v>4081</v>
       </c>
       <c r="G29" s="1">
@@ -1853,7 +1925,7 @@
         <v>10093</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f>E30-D30+1</f>
         <v>1440</v>
       </c>
       <c r="G30" s="1">
@@ -1880,7 +1952,7 @@
         <v>10049</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f>E31-D31+1</f>
         <v>1369</v>
       </c>
       <c r="G31" s="1">
@@ -1907,7 +1979,7 @@
         <v>11096</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f>E32-D32+1</f>
         <v>1095</v>
       </c>
       <c r="G32" s="1">
@@ -1934,7 +2006,7 @@
         <v>11079</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f>E33-D33+1</f>
         <v>979</v>
       </c>
       <c r="G33" s="1">
@@ -1961,7 +2033,7 @@
         <v>11088</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f>E34-D34+1</f>
         <v>997</v>
       </c>
       <c r="G34" s="1">
@@ -1988,7 +2060,7 @@
         <v>12090</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f>E35-D35+1</f>
         <v>1047</v>
       </c>
       <c r="G35" s="1">
@@ -2015,7 +2087,7 @@
         <v>12046</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f>E36-D36+1</f>
         <v>781</v>
       </c>
       <c r="G36" s="1">
@@ -2083,6 +2155,139 @@
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1654</v>
+      </c>
+      <c r="F39">
+        <v>1654</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40" s="4">
+        <v>1544</v>
+      </c>
+      <c r="F40" s="4">
+        <v>1537</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1923</v>
+      </c>
+      <c r="E41" s="4">
+        <v>3260</v>
+      </c>
+      <c r="F41" s="4">
+        <v>1338</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="6">
+        <v>2127</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3171</v>
+      </c>
+      <c r="F42">
+        <f>Table1[[#This Row],[Maximum]]-Table1[[#This Row],[Minimum]]</f>
+        <v>1044</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>